<commit_message>
Make origin field to be dinamic
</commit_message>
<xml_diff>
--- a/uploads/28-6-2021-prueba_con_1_lead.xlsx
+++ b/uploads/28-6-2021-prueba_con_1_lead.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documentos\WePlan\side-projects\XAPPIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5A3277A-1999-4988-858E-4C1EE27CFA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2558C29C-8E86-404F-A17E-21084D435360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{EFF83964-08C8-4D72-8D45-5FBD567118BF}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{EFF83964-08C8-4D72-8D45-5FBD567118BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>NOMBRE-APELLIDO</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Le interesa el Corolla, cuenta con un chevrolet tracker mod 2014. Horario de contacto 17:30hs</t>
+  </si>
+  <si>
+    <t>ORIGEN</t>
+  </si>
+  <si>
+    <t>AGP AMBA</t>
   </si>
 </sst>
 </file>
@@ -89,7 +95,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -125,11 +131,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -139,6 +156,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE4CD761-454B-4C07-84A5-9006A2F4D5D2}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +485,7 @@
     <col min="5" max="5" width="80.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,8 +501,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -497,6 +518,9 @@
       </c>
       <c r="E2" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>